<commit_message>
Null model 2 Updated
</commit_message>
<xml_diff>
--- a/Results/Jac/Table_models.xlsx
+++ b/Results/Jac/Table_models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agustin/Desktop/Papers/Canary_Island_Project/spatial_modularity_in_the_canary_islands/Results/Jac/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A548A37-81F4-4B40-A2C3-633DED2D6ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7530A531-F07C-114D-9094-45E1F64AF0A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10460" yWindow="1140" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{EB4D4A07-8EA4-EE43-B3EA-B2E3F1412D83}"/>
+    <workbookView xWindow="10360" yWindow="1140" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{EB4D4A07-8EA4-EE43-B3EA-B2E3F1412D83}"/>
   </bookViews>
   <sheets>
     <sheet name="M1_ave_species" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="15">
   <si>
     <t>Model</t>
   </si>
@@ -707,7 +707,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="A2:F5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -752,7 +752,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.2">
@@ -825,7 +825,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+      <selection activeCell="A2" sqref="A2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -858,13 +858,13 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="C2" s="3">
-        <v>-7.6817380000000005E-7</v>
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-1E-3</v>
       </c>
       <c r="D2" s="2">
-        <v>0.65</v>
+        <v>0.53800000000000003</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>5</v>
@@ -878,16 +878,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="2">
-        <v>0.22</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="C3" s="3">
-        <v>-3.467E-7</v>
+        <v>-1.1000000000000001E-3</v>
       </c>
       <c r="D3" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="E3" s="8">
-        <v>6.0000000000000001E-3</v>
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="F3" s="2">
         <v>19</v>
@@ -910,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D50903-B655-604E-A4B6-C33E0B5414BE}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8:U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -941,13 +941,13 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="C2" s="3">
-        <v>-7.6817380000000005E-7</v>
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-1E-3</v>
       </c>
       <c r="D2" s="2">
-        <v>0.65</v>
+        <v>0.53800000000000003</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>5</v>
@@ -961,16 +961,16 @@
         <v>13</v>
       </c>
       <c r="B3" s="2">
-        <v>0.12</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="C3" s="3">
-        <v>-4.7250000000000003E-8</v>
+        <v>-5.3820000000000003E-5</v>
       </c>
       <c r="D3" s="2">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0.124</v>
+        <v>0.6</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="F3" s="2">
         <v>19</v>
@@ -1316,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86507568-4B9D-774E-B406-B889FB677538}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1359,7 +1359,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.2">
@@ -1427,16 +1427,16 @@
         <v>12</v>
       </c>
       <c r="B6" s="2">
-        <v>0.22</v>
+        <v>0.57599999999999996</v>
       </c>
       <c r="C6" s="3">
-        <v>-3.467E-7</v>
+        <v>-1.1000000000000001E-3</v>
       </c>
       <c r="D6" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="E6" s="8">
-        <v>6.0000000000000001E-3</v>
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="F6" s="2">
         <v>19</v>

</xml_diff>